<commit_message>
update file for suffer
</commit_message>
<xml_diff>
--- a/Nam3_HK1/CSDL_SQL_Plus/Baitap/Tuan10/BTap.xlsx
+++ b/Nam3_HK1/CSDL_SQL_Plus/Baitap/Tuan10/BTap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SGU-Course\Nam3_HK1\CSDL_SQL_Plus\Baitap\Tuan10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A10BFE-B616-4792-AF9F-0926E3093C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3067C86F-F616-4F15-823E-B5BAD3F57807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{88E02BB5-18DC-4D8D-A50A-9D70CEF122C2}"/>
   </bookViews>
@@ -467,19 +467,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7EAA01-9FA6-4241-AC58-07A4C2D419DD}">
-  <dimension ref="A29:M39"/>
+  <dimension ref="A29:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="25.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="40.88671875" style="1" customWidth="1"/>
     <col min="11" max="12" width="25.77734375" style="1" customWidth="1"/>
     <col min="13" max="13" width="42.88671875" style="1" customWidth="1"/>
@@ -489,7 +493,7 @@
     <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
@@ -505,32 +509,8 @@
       <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>150</v>
       </c>
@@ -546,173 +526,219 @@
       <c r="E30" s="3">
         <v>30000</v>
       </c>
-      <c r="F30" s="3">
-        <f>ROUND(B30/A30, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="G30" s="3">
-        <f>ROUND(E30/F30, 0)</f>
-        <v>10000</v>
-      </c>
-      <c r="H30" s="3">
-        <f>D30+C30</f>
-        <v>16</v>
-      </c>
-      <c r="I30" s="3">
-        <f>ROUND(B30/H30, 0)</f>
-        <v>32</v>
-      </c>
-      <c r="J30" s="3">
-        <f>ROUND(E30/I30, 0)</f>
-        <v>938</v>
-      </c>
-      <c r="K30" s="3">
-        <f>ROUND(LOG(J30, 2), 0)+1</f>
-        <v>11</v>
-      </c>
-      <c r="L30" s="3">
-        <f>G30/2</f>
-        <v>5000</v>
-      </c>
-      <c r="M30" s="3">
-        <f>ROUND(LOG(G30,2), 0)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <f>ROUND(B30/A30, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="B46" s="3">
+        <f>ROUND(E30/A46, 0)</f>
+        <v>10000</v>
+      </c>
+      <c r="C46" s="3">
+        <f>D30+C30</f>
+        <v>16</v>
+      </c>
+      <c r="D46" s="3">
+        <f>ROUND(B30/C46, 0)</f>
+        <v>32</v>
+      </c>
+      <c r="E46" s="3">
+        <f>ROUND(E30/D46, 0)</f>
+        <v>938</v>
+      </c>
+      <c r="F46" s="3">
+        <f>ROUND(LOG(E46, 2), 0)+1</f>
+        <v>11</v>
+      </c>
+      <c r="G46" s="3">
+        <f>B46/2</f>
+        <v>5000</v>
+      </c>
+      <c r="H46" s="3">
+        <f>ROUND(LOG(B46,2), 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>